<commit_message>
upload figures png and delete fig files from github
</commit_message>
<xml_diff>
--- a/figures/results_figures/results_array.xlsx
+++ b/figures/results_figures/results_array.xlsx
@@ -750,8 +750,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1460,7 +1461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1579,6 +1580,27 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1594,10 +1616,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1648,10 +1670,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1778,8 +1800,122 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$39:$M$50</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Uadd/F=2.5%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Uadd/F=2.5%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Uadd/F=2.5%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Uadd/F=2.5%, Umul=100%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Uadd/F=5%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Uadd/F=5%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Uadd/F=5%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Uadd/F=5%, Umul=100%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Uadd/F=10%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Uadd/F=10%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Uadd/F=10%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Uadd/F=10%, Umul=100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$14:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.44650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36070000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24490000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25540000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2223</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2382</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21360000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$L$20</c:f>
@@ -1803,44 +1939,44 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$45:$M$56</c:f>
+              <c:f>Sheet1!$M$39:$M$50</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Uadd/F=2.5%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Uadd/F=2.5%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Uadd/F=2.5%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Uadd/F=2.5%, Umul=100%</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>Uadd/F=2.5%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Uadd/F=2.5%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Uadd/F=2.5%, Umul=75%</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>Uadd/F=5%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Uadd/F=5%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Uadd/F=5%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Uadd/F=5%, Umul=100%</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Uadd/F=5%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Uadd/F=5%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Uadd/F=5%, Umul=75%</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>Uadd/F=10%, Umul=25%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Uadd/F=10%, Umul=50%</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Uadd/F=10%, Umul=75%</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Uadd/F=10%, Umul=100%</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Uadd/F=10%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Uadd/F=10%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Uadd/F=10%, Umul=75%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1852,154 +1988,40 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.23662715653896385</c:v>
+                  <c:v>0.43469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25430628135515548</c:v>
+                  <c:v>0.28210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28209198735593172</c:v>
+                  <c:v>0.25430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4346737251627345</c:v>
+                  <c:v>0.2366</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22757402542791436</c:v>
+                  <c:v>0.35060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25307875592278495</c:v>
+                  <c:v>0.25330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25328987171553047</c:v>
+                  <c:v>0.25309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35058631536972962</c:v>
+                  <c:v>0.2276</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21835410708760961</c:v>
+                  <c:v>0.22239999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2186278463793149</c:v>
+                  <c:v>0.2162</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21617848532292275</c:v>
+                  <c:v>0.21859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22244895886172322</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$L$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$M$45:$M$56</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Uadd/F=2.5%, Umul=100%</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Uadd/F=2.5%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Uadd/F=2.5%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Uadd/F=2.5%, Umul=75%</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uadd/F=5%, Umul=100%</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Uadd/F=5%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Uadd/F=5%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Uadd/F=5%, Umul=75%</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Uadd/F=10%, Umul=100%</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Uadd/F=10%, Umul=25%</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Uadd/F=10%, Umul=50%</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Uadd/F=10%, Umul=75%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$14:$H$25</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.23515118391183359</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27003164325034507</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27281432544372014</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.44646168495043886</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.25540375772678275</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.23670167995704142</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.24489091941725288</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.36071223032900623</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2135947348883834</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.23824443118522126</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.22229126897898754</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.22836388132433222</c:v>
+                  <c:v>0.21840000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,11 +2036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256854192"/>
-        <c:axId val="256856544"/>
+        <c:axId val="361490776"/>
+        <c:axId val="361491952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256854192"/>
+        <c:axId val="361490776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2061,7 +2083,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256856544"/>
+        <c:crossAx val="361491952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2069,7 +2091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256856544"/>
+        <c:axId val="361491952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2198,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256854192"/>
+        <c:crossAx val="361490776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2327,21 +2349,21 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2353,16 +2375,98 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23662715653896385</c:v>
+                  <c:v>0.43469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25430628135515548</c:v>
+                  <c:v>0.28210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28209198735593172</c:v>
+                  <c:v>0.25430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4346737251627345</c:v>
+                  <c:v>0.2366</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=5, Uadd/F=2.5%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$14:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.44650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23519999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2371,7 +2475,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$M$62</c:f>
@@ -2409,21 +2513,21 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2435,16 +2539,98 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.22757402542791436</c:v>
+                  <c:v>0.35060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25307875592278495</c:v>
+                  <c:v>0.25330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25328987171553047</c:v>
+                  <c:v>0.25309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35058631536972962</c:v>
+                  <c:v>0.2276</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=5, Uadd/F=5%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$18:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.36070000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24490000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25540000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2453,7 +2639,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$M$63</c:f>
@@ -2491,21 +2677,21 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2517,180 +2703,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.21835410708760961</c:v>
+                  <c:v>0.22239999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2186278463793149</c:v>
+                  <c:v>0.2162</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21617848532292275</c:v>
+                  <c:v>0.21859999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22244895886172322</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$64</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=5, Uadd/F=2.5%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$14:$H$17</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.23515118391183359</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27003164325034507</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27281432544372014</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.44646168495043886</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$M$65</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=5, Uadd/F=5%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$18:$H$21</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.25540375772678275</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23670167995704142</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24489091941725288</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.36071223032900623</c:v>
+                  <c:v>0.21840000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2737,21 +2759,21 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>Sheet1!$J$24:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2763,16 +2785,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.2135947348883834</c:v>
+                  <c:v>0.22839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23824443118522126</c:v>
+                  <c:v>0.2223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22229126897898754</c:v>
+                  <c:v>0.2382</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22836388132433222</c:v>
+                  <c:v>0.21360000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2789,11 +2811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="256849880"/>
-        <c:axId val="256855760"/>
+        <c:axId val="361488032"/>
+        <c:axId val="361493912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="256849880"/>
+        <c:axId val="361488032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2926,7 +2948,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256855760"/>
+        <c:crossAx val="361493912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2934,7 +2956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256855760"/>
+        <c:axId val="361493912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3042,7 +3064,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256849880"/>
+        <c:crossAx val="361488032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3628,12 +3650,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="256850272"/>
-        <c:axId val="256852624"/>
-        <c:axId val="257666808"/>
+        <c:axId val="361496656"/>
+        <c:axId val="361509592"/>
+        <c:axId val="363516856"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="256850272"/>
+        <c:axId val="361496656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3728,7 +3750,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256852624"/>
+        <c:crossAx val="361509592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3736,7 +3758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256852624"/>
+        <c:axId val="361509592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3840,12 +3862,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256850272"/>
+        <c:crossAx val="361496656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="257666808"/>
+        <c:axId val="363516856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3939,7 +3961,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256852624"/>
+        <c:crossAx val="361509592"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -4155,8 +4177,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10726498893520663"/>
-          <c:y val="1.8242526489369418E-2"/>
+          <c:x val="0.11185634689294101"/>
+          <c:y val="3.4165282372860054E-2"/>
           <c:w val="0.84701332921620087"/>
           <c:h val="0.86063004509857022"/>
         </c:manualLayout>
@@ -4165,15 +4187,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$2</c:f>
+              <c:f>Sheet1!$N$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>σ=2, Umul=100%</c:v>
+                  <c:v>σ=2, Umul=25%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4181,7 +4203,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4192,11 +4214,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4204,36 +4226,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$10,Sheet1!$H$6,Sheet1!$H$2)</c:f>
+              <c:f>(Sheet1!$H$2,Sheet1!$H$6,Sheet1!$H$10)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.21835410708760961</c:v>
+                  <c:v>0.43469999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22757402542791436</c:v>
+                  <c:v>0.35060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23662715653896385</c:v>
+                  <c:v>0.22239999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4241,15 +4263,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="7"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$3</c:f>
+              <c:f>Sheet1!$N$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>σ=2, Umul=75%</c:v>
+                  <c:v>σ=5, Umul=25%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4257,7 +4279,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4268,11 +4292,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4280,36 +4308,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$11,Sheet1!$H$7,Sheet1!$H$3)</c:f>
+              <c:f>(Sheet1!$H$14,Sheet1!$H$18,Sheet1!$H$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.2186278463793149</c:v>
+                  <c:v>0.44650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25307875592278495</c:v>
+                  <c:v>0.36070000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25430628135515548</c:v>
+                  <c:v>0.22839999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4356,264 +4384,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$12,Sheet1!$H$8,Sheet1!$H$4)</c:f>
+              <c:f>(Sheet1!$H$3,Sheet1!$H$7,Sheet1!$H$11)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.21617848532292275</c:v>
+                  <c:v>0.28210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25328987171553047</c:v>
+                  <c:v>0.25330000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28209198735593172</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=2, Umul=25%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$H$13,Sheet1!$H$9,Sheet1!$H$5)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.22244895886172322</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.35058631536972962</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4346737251627345</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=5, Umul=100%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$H$22,Sheet1!$H$18,Sheet1!$H$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.2135947348883834</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25540375772678275</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23515118391183359</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>σ=5, Umul=75%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$H$23,Sheet1!$H$19,Sheet1!$H$15)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.23824443118522126</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23670167995704142</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27003164325034507</c:v>
+                  <c:v>0.2162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4622,7 +4422,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$N$8</c:f>
@@ -4666,36 +4466,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$24,Sheet1!$H$20,Sheet1!$H$16)</c:f>
+              <c:f>(Sheet1!$H$15,Sheet1!$H$19,Sheet1!$H$23)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.22229126897898754</c:v>
+                  <c:v>0.27279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24489091941725288</c:v>
+                  <c:v>0.24490000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27281432544372014</c:v>
+                  <c:v>0.2223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4703,15 +4503,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:idx val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$9</c:f>
+              <c:f>Sheet1!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>σ=5, Umul=25%</c:v>
+                  <c:v>σ=2, Umul=75%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4719,9 +4519,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4732,15 +4530,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -4748,36 +4542,264 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>(Sheet1!$D$22,Sheet1!$D$18,Sheet1!$D$14)</c:f>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$H$25,Sheet1!$H$21,Sheet1!$H$17)</c:f>
+              <c:f>(Sheet1!$H$4,Sheet1!$H$8,Sheet1!$H$12)</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.22836388132433222</c:v>
+                  <c:v>0.25430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36071223032900623</c:v>
+                  <c:v>0.25309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44646168495043886</c:v>
+                  <c:v>0.21859999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=5, Umul=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$H$16,Sheet1!$H$20,Sheet1!$H$24)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=2, Umul=100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$H$5,Sheet1!$H$9,Sheet1!$H$13)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.2366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2276</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21840000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>σ=5, Umul=100%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$D$14,Sheet1!$D$18,Sheet1!$D$22)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$H$17,Sheet1!$H$21,Sheet1!$H$25)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.23519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25540000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21360000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4794,11 +4816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="256854976"/>
-        <c:axId val="256851448"/>
+        <c:axId val="361510768"/>
+        <c:axId val="361514688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="256854976"/>
+        <c:axId val="361510768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4905,7 +4927,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256851448"/>
+        <c:crossAx val="361514688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4913,7 +4935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256851448"/>
+        <c:axId val="361514688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.48000000000000004"/>
@@ -5029,7 +5051,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256854976"/>
+        <c:crossAx val="361510768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6799,16 +6821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>300556</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>160162</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>768146</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>73571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>176893</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>32817</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>679119</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>136726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7296,15 +7318,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>326570</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:colOff>382600</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>92048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>167368</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>5603</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>189780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7589,10 +7611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:AP66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7607,10 +7629,12 @@
     <col min="9" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="17" width="1.42578125" customWidth="1"/>
+    <col min="16" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="42" width="10.7109375" customWidth="1"/>
+    <col min="43" max="79" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39"/>
       <c r="B1" s="38" t="s">
         <v>8</v>
@@ -7644,31 +7668,30 @@
       <c r="N1"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46">
+    <row r="2" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53">
         <v>0.05</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="60">
         <v>11</v>
       </c>
-      <c r="C2" s="56">
+      <c r="C2" s="63">
         <v>2</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E2" s="40">
-        <v>1</v>
-      </c>
-      <c r="F2" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="63">
         <v>2004</v>
       </c>
-      <c r="G2" s="63">
+      <c r="G2" s="70">
         <v>182</v>
       </c>
       <c r="H2" s="23">
-        <f>$O2/100</f>
-        <v>0.23662715653896385</v>
+        <v>0.43469999999999998</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>0</v>
@@ -7692,19 +7715,18 @@
         <v>23.662715653896385</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+    <row r="3" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="57"/>
+      <c r="G3" s="71"/>
       <c r="H3" s="24">
-        <f t="shared" ref="H3:H34" si="0">$O3/100</f>
-        <v>0.25430628135515548</v>
+        <v>0.28210000000000002</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>1</v>
@@ -7728,19 +7750,18 @@
         <v>25.430628135515548</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+    <row r="4" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="57"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="24">
-        <f t="shared" si="0"/>
-        <v>0.28209198735593172</v>
+        <v>0.25430000000000003</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>2</v>
@@ -7764,19 +7785,18 @@
         <v>28.209198735593169</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+    <row r="5" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="57"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="28">
-        <f t="shared" si="0"/>
-        <v>0.4346737251627345</v>
+        <v>0.2366</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>3</v>
@@ -7800,21 +7820,20 @@
         <v>43.46737251627345</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="49">
+    <row r="6" spans="1:42" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="56">
         <v>0.05</v>
       </c>
       <c r="E6" s="40">
-        <v>1</v>
-      </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="64"/>
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="57"/>
+      <c r="G6" s="71"/>
       <c r="H6" s="29">
-        <f t="shared" si="0"/>
-        <v>0.22757402542791436</v>
+        <v>0.35060000000000002</v>
       </c>
       <c r="N6" s="45" t="s">
         <v>37</v>
@@ -7823,19 +7842,18 @@
         <v>22.757402542791436</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
+    <row r="7" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="57"/>
+      <c r="G7" s="71"/>
       <c r="H7" s="26">
-        <f t="shared" si="0"/>
-        <v>0.25307875592278495</v>
+        <v>0.25330000000000003</v>
       </c>
       <c r="N7" s="45" t="s">
         <v>38</v>
@@ -7844,19 +7862,18 @@
         <v>25.307875592278492</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+    <row r="8" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="54"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="50"/>
-      <c r="G8" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="57"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="24">
-        <f t="shared" si="0"/>
-        <v>0.25328987171553047</v>
+        <v>0.25309999999999999</v>
       </c>
       <c r="N8" s="45" t="s">
         <v>39</v>
@@ -7865,19 +7882,18 @@
         <v>25.328987171553045</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="52"/>
+    <row r="9" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="54"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="57"/>
+      <c r="G9" s="71"/>
       <c r="H9" s="27">
-        <f t="shared" si="0"/>
-        <v>0.35058631536972962</v>
+        <v>0.2276</v>
       </c>
       <c r="N9" s="45" t="s">
         <v>40</v>
@@ -7885,60 +7901,153 @@
       <c r="O9" s="4">
         <v>35.05863153697296</v>
       </c>
+      <c r="S9" s="46">
+        <f>$O2/100</f>
+        <v>0.23662715653896385</v>
+      </c>
+      <c r="T9" s="47">
+        <f>$O3/100</f>
+        <v>0.25430628135515548</v>
+      </c>
+      <c r="U9" s="47">
+        <f>$O4/100</f>
+        <v>0.28209198735593172</v>
+      </c>
+      <c r="V9" s="48">
+        <f>$O5/100</f>
+        <v>0.4346737251627345</v>
+      </c>
+      <c r="W9" s="49">
+        <f>$O6/100</f>
+        <v>0.22757402542791436</v>
+      </c>
+      <c r="X9" s="50">
+        <f>$O7/100</f>
+        <v>0.25307875592278495</v>
+      </c>
+      <c r="Y9" s="47">
+        <f>$O8/100</f>
+        <v>0.25328987171553047</v>
+      </c>
+      <c r="Z9" s="51">
+        <f>$O9/100</f>
+        <v>0.35058631536972962</v>
+      </c>
+      <c r="AA9" s="49">
+        <f>$O10/100</f>
+        <v>0.21835410708760961</v>
+      </c>
+      <c r="AB9" s="47">
+        <f>$O11/100</f>
+        <v>0.2186278463793149</v>
+      </c>
+      <c r="AC9" s="47">
+        <f>$O12/100</f>
+        <v>0.21617848532292275</v>
+      </c>
+      <c r="AD9" s="52">
+        <f>$O13/100</f>
+        <v>0.22244895886172322</v>
+      </c>
+      <c r="AE9" s="46">
+        <f>$O14/100</f>
+        <v>0.23515118391183359</v>
+      </c>
+      <c r="AF9" s="47">
+        <f>$O15/100</f>
+        <v>0.27003164325034507</v>
+      </c>
+      <c r="AG9" s="47">
+        <f>$O16/100</f>
+        <v>0.27281432544372014</v>
+      </c>
+      <c r="AH9" s="51">
+        <f>$O17/100</f>
+        <v>0.44646168495043886</v>
+      </c>
+      <c r="AI9" s="49">
+        <f>$O18/100</f>
+        <v>0.25540375772678275</v>
+      </c>
+      <c r="AJ9" s="47">
+        <f>$O20/100</f>
+        <v>0.23670167995704142</v>
+      </c>
+      <c r="AK9" s="47">
+        <f>$O19/100</f>
+        <v>0.24489091941725288</v>
+      </c>
+      <c r="AL9" s="51">
+        <f>$O21/100</f>
+        <v>0.36071223032900623</v>
+      </c>
+      <c r="AM9" s="49">
+        <f>$O22/100</f>
+        <v>0.2135947348883834</v>
+      </c>
+      <c r="AN9" s="47">
+        <f>$O23/100</f>
+        <v>0.23824443118522126</v>
+      </c>
+      <c r="AO9" s="47">
+        <f>$O24/100</f>
+        <v>0.22229126897898754</v>
+      </c>
+      <c r="AP9" s="48">
+        <f>$O25/100</f>
+        <v>0.22836388132433222</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="69">
+    <row r="10" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="59">
         <v>0.1</v>
       </c>
       <c r="E10" s="40">
-        <v>1</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="64"/>
+        <v>0.25</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="29">
-        <f t="shared" si="0"/>
-        <v>0.21835410708760961</v>
+        <v>0.22239999999999999</v>
       </c>
       <c r="N10"/>
       <c r="O10" s="4">
         <v>21.835410708760961</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
+    <row r="11" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="24">
-        <f t="shared" si="0"/>
-        <v>0.2186278463793149</v>
+        <v>0.2162</v>
       </c>
       <c r="N11"/>
       <c r="O11" s="4">
         <v>21.86278463793149</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
+    <row r="12" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="71"/>
       <c r="H12" s="24">
-        <f t="shared" si="0"/>
-        <v>0.21617848532292275</v>
+        <v>0.21859999999999999</v>
       </c>
       <c r="I12" s="8"/>
       <c r="N12"/>
@@ -7946,19 +8055,18 @@
         <v>21.617848532292275</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+    <row r="13" spans="1:42" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="54"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="57"/>
+      <c r="G13" s="71"/>
       <c r="H13" s="30">
-        <f t="shared" si="0"/>
-        <v>0.22244895886172322</v>
+        <v>0.21840000000000001</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>5</v>
@@ -7977,23 +8085,22 @@
         <v>22.244895886172323</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="56">
+    <row r="14" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="63">
         <v>5</v>
       </c>
-      <c r="D14" s="49">
+      <c r="D14" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E14" s="40">
-        <v>1</v>
-      </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="64"/>
+        <v>0.25</v>
+      </c>
+      <c r="F14" s="57"/>
+      <c r="G14" s="71"/>
       <c r="H14" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23515118391183359</v>
+        <v>0.44650000000000001</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>0</v>
@@ -8015,19 +8122,18 @@
         <v>23.515118391183361</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
+    <row r="15" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F15" s="50"/>
-      <c r="G15" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="71"/>
       <c r="H15" s="24">
-        <f t="shared" si="0"/>
-        <v>0.27003164325034507</v>
+        <v>0.27279999999999999</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>1</v>
@@ -8049,19 +8155,18 @@
         <v>27.003164325034504</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
+    <row r="16" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F16" s="57"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="24">
-        <f t="shared" si="0"/>
-        <v>0.27281432544372014</v>
+        <v>0.27</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>2</v>
@@ -8084,18 +8189,17 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="57"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="27">
-        <f t="shared" si="0"/>
-        <v>0.44646168495043886</v>
+        <v>0.23519999999999999</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>3</v>
@@ -8118,20 +8222,19 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="49">
+      <c r="A18" s="54"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="56">
         <v>0.05</v>
       </c>
       <c r="E18" s="40">
-        <v>1</v>
-      </c>
-      <c r="F18" s="50"/>
-      <c r="G18" s="64"/>
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="57"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="29">
-        <f t="shared" si="0"/>
-        <v>0.25540375772678275</v>
+        <v>0.36070000000000002</v>
       </c>
       <c r="N18"/>
       <c r="O18" s="4">
@@ -8139,18 +8242,17 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="57"/>
+      <c r="G19" s="71"/>
       <c r="H19" s="24">
-        <f>$O20/100</f>
-        <v>0.23670167995704142</v>
+        <v>0.24490000000000001</v>
       </c>
       <c r="L19" s="45" t="s">
         <v>14</v>
@@ -8161,18 +8263,17 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="24">
-        <f>$O19/100</f>
-        <v>0.24489091941725288</v>
+        <v>0.23669999999999999</v>
       </c>
       <c r="L20" s="45" t="s">
         <v>13</v>
@@ -8183,18 +8284,17 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
       <c r="E21" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="71"/>
       <c r="H21" s="27">
-        <f t="shared" si="0"/>
-        <v>0.36071223032900623</v>
+        <v>0.25540000000000002</v>
       </c>
       <c r="L21" s="45" t="s">
         <v>11</v>
@@ -8205,20 +8305,19 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="3.5">
-      <c r="A22" s="47"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="69">
+      <c r="A22" s="54"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="59">
         <v>0.1</v>
       </c>
       <c r="E22" s="40">
-        <v>1</v>
-      </c>
-      <c r="F22" s="50"/>
-      <c r="G22" s="64"/>
+        <v>0.25</v>
+      </c>
+      <c r="F22" s="57"/>
+      <c r="G22" s="71"/>
       <c r="H22" s="29">
-        <f>$O22/100</f>
-        <v>0.2135947348883834</v>
+        <v>0.22839999999999999</v>
       </c>
       <c r="L22" s="44" t="s">
         <v>12</v>
@@ -8229,18 +8328,17 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="64"/>
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="57"/>
+      <c r="G23" s="71"/>
       <c r="H23" s="24">
-        <f t="shared" si="0"/>
-        <v>0.23824443118522126</v>
+        <v>0.2223</v>
       </c>
       <c r="N23"/>
       <c r="O23" s="4">
@@ -8248,18 +8346,20 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="F24" s="50"/>
-      <c r="G24" s="64"/>
+        <v>0.75</v>
+      </c>
+      <c r="F24" s="57"/>
+      <c r="G24" s="71"/>
       <c r="H24" s="24">
-        <f t="shared" si="0"/>
-        <v>0.22229126897898754</v>
+        <v>0.2382</v>
+      </c>
+      <c r="J24" s="42">
+        <v>0.25</v>
       </c>
       <c r="N24"/>
       <c r="O24" s="4">
@@ -8267,47 +8367,52 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="68"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="58"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="28">
-        <f t="shared" si="0"/>
-        <v>0.22836388132433222</v>
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="J25" s="41">
+        <v>0.5</v>
       </c>
       <c r="N25"/>
       <c r="O25" s="4">
         <v>22.836388132433221</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="57">
+    <row r="26" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
+      <c r="B26" s="64">
         <v>12</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="63">
         <v>2</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E26" s="72">
+      <c r="E26" s="79">
         <v>0.5</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F26" s="63">
         <v>3002</v>
       </c>
-      <c r="G26" s="63">
+      <c r="G26" s="70">
         <v>250</v>
       </c>
       <c r="H26" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H26:H34" si="0">$O26/100</f>
         <v>0.27101494242150292</v>
+      </c>
+      <c r="J26" s="41">
+        <v>0.75</v>
       </c>
       <c r="N26"/>
       <c r="O26" s="4">
@@ -8315,30 +8420,33 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="64"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="71"/>
       <c r="H27" s="36">
         <f t="shared" si="0"/>
         <v>0.27767733150117957</v>
       </c>
+      <c r="J27" s="40">
+        <v>1</v>
+      </c>
       <c r="N27"/>
       <c r="O27" s="4">
         <v>27.767733150117959</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="65"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="72"/>
       <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>0.27747258302453448</v>
@@ -8349,17 +8457,17 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="60">
+      <c r="A29" s="54"/>
+      <c r="B29" s="67">
         <v>24</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="71">
+      <c r="C29" s="57"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="78">
         <v>3002</v>
       </c>
-      <c r="G29" s="66">
+      <c r="G29" s="73">
         <v>125</v>
       </c>
       <c r="H29" s="29">
@@ -8372,13 +8480,13 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="64"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="71"/>
       <c r="H30" s="24">
         <f t="shared" si="0"/>
         <v>0.27066461952200482</v>
@@ -8389,13 +8497,13 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="65"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="72"/>
       <c r="H31" s="27">
         <f t="shared" si="0"/>
         <v>0.27348055020385287</v>
@@ -8406,17 +8514,17 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="60">
+      <c r="A32" s="54"/>
+      <c r="B32" s="67">
         <v>36</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="71">
+      <c r="C32" s="57"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="78">
         <v>3026</v>
       </c>
-      <c r="G32" s="66">
+      <c r="G32" s="73">
         <v>84</v>
       </c>
       <c r="H32" s="26">
@@ -8429,13 +8537,13 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="64"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="71"/>
       <c r="H33" s="24">
         <f t="shared" si="0"/>
         <v>0.27125796408372016</v>
@@ -8446,13 +8554,13 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="67"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="74"/>
       <c r="H34" s="25">
         <f t="shared" si="0"/>
         <v>0.27194846949300938</v>
@@ -8462,64 +8570,64 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="45" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M52" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M53" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M54" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M55" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="M56" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
first draft for polytechnique without conclusion finished. Todo : Conclusion, reposition figures, improve aspect, reread and modify 1000 times.
</commit_message>
<xml_diff>
--- a/figures/results_figures/results_array.xlsx
+++ b/figures/results_figures/results_array.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3075" windowHeight="1755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="3075" windowHeight="1755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1601,57 +1601,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1670,13 +1619,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1686,6 +1653,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2036,11 +2036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="361490776"/>
-        <c:axId val="361491952"/>
+        <c:axId val="328656160"/>
+        <c:axId val="328656552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361490776"/>
+        <c:axId val="328656160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2083,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361491952"/>
+        <c:crossAx val="328656552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2091,7 +2091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361491952"/>
+        <c:axId val="328656552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2198,7 +2198,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361490776"/>
+        <c:crossAx val="328656160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2811,11 +2811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361488032"/>
-        <c:axId val="361493912"/>
+        <c:axId val="328660472"/>
+        <c:axId val="328660864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361488032"/>
+        <c:axId val="328660472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2878,7 +2878,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2948,7 +2947,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361493912"/>
+        <c:crossAx val="328660864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2956,7 +2955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361493912"/>
+        <c:axId val="328660864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3003,7 +3002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3064,7 +3062,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361488032"/>
+        <c:crossAx val="328660472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3078,7 +3076,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3650,12 +3647,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="361496656"/>
-        <c:axId val="361509592"/>
-        <c:axId val="363516856"/>
+        <c:axId val="100259904"/>
+        <c:axId val="100260688"/>
+        <c:axId val="282369208"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="361496656"/>
+        <c:axId val="100259904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3750,7 +3747,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361509592"/>
+        <c:crossAx val="100260688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3758,7 +3755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361509592"/>
+        <c:axId val="100260688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3862,12 +3859,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361496656"/>
+        <c:crossAx val="100259904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="363516856"/>
+        <c:axId val="282369208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3961,7 +3958,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361509592"/>
+        <c:crossAx val="100260688"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -4816,11 +4813,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361510768"/>
-        <c:axId val="361514688"/>
+        <c:axId val="100256376"/>
+        <c:axId val="100257552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361510768"/>
+        <c:axId val="100256376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4860,7 +4857,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4927,7 +4923,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361514688"/>
+        <c:crossAx val="100257552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4935,7 +4931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361514688"/>
+        <c:axId val="100257552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.48000000000000004"/>
@@ -5051,7 +5047,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361510768"/>
+        <c:crossAx val="100256376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5065,7 +5061,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7613,8 +7608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:H34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7669,25 +7664,25 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53">
+      <c r="A2" s="71">
         <v>0.05</v>
       </c>
-      <c r="B2" s="60">
+      <c r="B2" s="74">
         <v>11</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="62">
         <v>2</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="59">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E2" s="40">
         <v>0.25</v>
       </c>
-      <c r="F2" s="63">
+      <c r="F2" s="62">
         <v>2004</v>
       </c>
-      <c r="G2" s="70">
+      <c r="G2" s="53">
         <v>182</v>
       </c>
       <c r="H2" s="23">
@@ -7716,15 +7711,15 @@
       </c>
     </row>
     <row r="3" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
       <c r="E3" s="41">
         <v>0.5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="71"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="24">
         <v>0.28210000000000002</v>
       </c>
@@ -7751,15 +7746,15 @@
       </c>
     </row>
     <row r="4" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="41">
         <v>0.75</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="71"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="24">
         <v>0.25430000000000003</v>
       </c>
@@ -7786,15 +7781,15 @@
       </c>
     </row>
     <row r="5" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="42">
         <v>1</v>
       </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="71"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="28">
         <v>0.2366</v>
       </c>
@@ -7821,17 +7816,17 @@
       </c>
     </row>
     <row r="6" spans="1:42" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="56">
+      <c r="A6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="59">
         <v>0.05</v>
       </c>
       <c r="E6" s="40">
         <v>0.25</v>
       </c>
-      <c r="F6" s="57"/>
-      <c r="G6" s="71"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="29">
         <v>0.35060000000000002</v>
       </c>
@@ -7843,15 +7838,15 @@
       </c>
     </row>
     <row r="7" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="41">
         <v>0.5</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="71"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="26">
         <v>0.25330000000000003</v>
       </c>
@@ -7863,15 +7858,15 @@
       </c>
     </row>
     <row r="8" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="41">
         <v>0.75</v>
       </c>
-      <c r="F8" s="57"/>
-      <c r="G8" s="71"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="24">
         <v>0.25309999999999999</v>
       </c>
@@ -7883,15 +7878,15 @@
       </c>
     </row>
     <row r="9" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="42">
         <v>1</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="71"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="27">
         <v>0.2276</v>
       </c>
@@ -7999,17 +7994,17 @@
       </c>
     </row>
     <row r="10" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="59">
+      <c r="A10" s="72"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="60">
         <v>0.1</v>
       </c>
       <c r="E10" s="40">
         <v>0.25</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="71"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="29">
         <v>0.22239999999999999</v>
       </c>
@@ -8019,15 +8014,15 @@
       </c>
     </row>
     <row r="11" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
       <c r="E11" s="41">
         <v>0.5</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="71"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="24">
         <v>0.2162</v>
       </c>
@@ -8037,15 +8032,15 @@
       </c>
     </row>
     <row r="12" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="41">
         <v>0.75</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="71"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="24">
         <v>0.21859999999999999</v>
       </c>
@@ -8056,15 +8051,15 @@
       </c>
     </row>
     <row r="13" spans="1:42" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
       <c r="E13" s="42">
         <v>1</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="71"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="30">
         <v>0.21840000000000001</v>
       </c>
@@ -8086,19 +8081,19 @@
       </c>
     </row>
     <row r="14" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="63">
+      <c r="A14" s="72"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="62">
         <v>5</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="59">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E14" s="40">
         <v>0.25</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="71"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="23">
         <v>0.44650000000000001</v>
       </c>
@@ -8123,15 +8118,15 @@
       </c>
     </row>
     <row r="15" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="41">
         <v>0.5</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="71"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="24">
         <v>0.27279999999999999</v>
       </c>
@@ -8156,15 +8151,15 @@
       </c>
     </row>
     <row r="16" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="41">
         <v>0.75</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="71"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="24">
         <v>0.27</v>
       </c>
@@ -8189,15 +8184,15 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="42">
         <v>1</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="71"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="54"/>
       <c r="H17" s="27">
         <v>0.23519999999999999</v>
       </c>
@@ -8222,17 +8217,17 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="56">
+      <c r="A18" s="72"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="59">
         <v>0.05</v>
       </c>
       <c r="E18" s="40">
         <v>0.25</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="71"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="29">
         <v>0.36070000000000002</v>
       </c>
@@ -8242,15 +8237,15 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="41">
         <v>0.5</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="71"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="24">
         <v>0.24490000000000001</v>
       </c>
@@ -8263,15 +8258,15 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="41">
         <v>0.75</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="71"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="24">
         <v>0.23669999999999999</v>
       </c>
@@ -8284,15 +8279,15 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
       <c r="E21" s="42">
         <v>1</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="71"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="27">
         <v>0.25540000000000002</v>
       </c>
@@ -8305,17 +8300,17 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="3.5">
-      <c r="A22" s="54"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="59">
+      <c r="A22" s="72"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="60">
         <v>0.1</v>
       </c>
       <c r="E22" s="40">
         <v>0.25</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="71"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="29">
         <v>0.22839999999999999</v>
       </c>
@@ -8328,15 +8323,15 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="41">
         <v>0.5</v>
       </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="71"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="24">
         <v>0.2223</v>
       </c>
@@ -8346,15 +8341,15 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
       <c r="E24" s="41">
         <v>0.75</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="71"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="24">
         <v>0.2382</v>
       </c>
@@ -8367,15 +8362,15 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
       <c r="E25" s="42">
         <v>1</v>
       </c>
-      <c r="F25" s="58"/>
-      <c r="G25" s="75"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="28">
         <v>0.21360000000000001</v>
       </c>
@@ -8388,23 +8383,23 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="64">
+      <c r="A26" s="72"/>
+      <c r="B26" s="77">
         <v>12</v>
       </c>
-      <c r="C26" s="63">
+      <c r="C26" s="62">
         <v>2</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="59">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="68">
         <v>0.5</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="62">
         <v>3002</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G26" s="53">
         <v>250</v>
       </c>
       <c r="H26" s="35">
@@ -8420,13 +8415,13 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="71"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="36">
         <f t="shared" si="0"/>
         <v>0.27767733150117957</v>
@@ -8440,13 +8435,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="72"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="55"/>
       <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>0.27747258302453448</v>
@@ -8457,17 +8452,17 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="67">
+      <c r="A29" s="72"/>
+      <c r="B29" s="80">
         <v>24</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="78">
+      <c r="C29" s="63"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="66">
         <v>3002</v>
       </c>
-      <c r="G29" s="73">
+      <c r="G29" s="56">
         <v>125</v>
       </c>
       <c r="H29" s="29">
@@ -8480,13 +8475,13 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="71"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="24">
         <f t="shared" si="0"/>
         <v>0.27066461952200482</v>
@@ -8497,13 +8492,13 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="72"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="55"/>
       <c r="H31" s="27">
         <f t="shared" si="0"/>
         <v>0.27348055020385287</v>
@@ -8514,17 +8509,17 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="67">
+      <c r="A32" s="72"/>
+      <c r="B32" s="80">
         <v>36</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="78">
+      <c r="C32" s="63"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="66">
         <v>3026</v>
       </c>
-      <c r="G32" s="73">
+      <c r="G32" s="56">
         <v>84</v>
       </c>
       <c r="H32" s="26">
@@ -8537,13 +8532,13 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="71"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="24">
         <f t="shared" si="0"/>
         <v>0.27125796408372016</v>
@@ -8554,13 +8549,13 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="55"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="74"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="57"/>
       <c r="H34" s="25">
         <f t="shared" si="0"/>
         <v>0.27194846949300938</v>
@@ -8665,16 +8660,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="G2:G25"/>
-    <mergeCell ref="D26:D34"/>
-    <mergeCell ref="F2:F25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="E26:E34"/>
     <mergeCell ref="A2:A34"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D9"/>
@@ -8689,6 +8674,16 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C26:C34"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="G2:G25"/>
+    <mergeCell ref="D26:D34"/>
+    <mergeCell ref="F2:F25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="E26:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
working on presentation.tex. Minor stuff corrected in the poly report. Added polytechnique_report.pdf to github.
</commit_message>
<xml_diff>
--- a/figures/results_figures/results_array.xlsx
+++ b/figures/results_figures/results_array.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="3075" windowHeight="1755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3075" windowHeight="1755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,30 +65,6 @@
   </si>
   <si>
     <t>Initial standard deviation : σ</t>
-  </si>
-  <si>
-    <r>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>CP</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> minimum : J*</t>
-    </r>
   </si>
   <si>
     <t>λ</t>
@@ -745,6 +721,9 @@
       <t>=25%</t>
     </r>
   </si>
+  <si>
+    <t>J minimum : J*</t>
+  </si>
 </sst>
 </file>
 
@@ -754,7 +733,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,13 +760,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="subscript"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1575,10 +1547,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1601,91 +1573,91 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2036,11 +2008,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="328656160"/>
-        <c:axId val="328656552"/>
+        <c:axId val="282126656"/>
+        <c:axId val="282125088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="328656160"/>
+        <c:axId val="282126656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2055,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328656552"/>
+        <c:crossAx val="282125088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2091,7 +2063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328656552"/>
+        <c:axId val="282125088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2198,7 +2170,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328656160"/>
+        <c:crossAx val="282126656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2811,11 +2783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="328660472"/>
-        <c:axId val="328660864"/>
+        <c:axId val="354175808"/>
+        <c:axId val="354176592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="328660472"/>
+        <c:axId val="354175808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2947,7 +2919,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328660864"/>
+        <c:crossAx val="354176592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2955,7 +2927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328660864"/>
+        <c:axId val="354176592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3062,7 +3034,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328660472"/>
+        <c:crossAx val="354175808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3647,12 +3619,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="100259904"/>
-        <c:axId val="100260688"/>
-        <c:axId val="282369208"/>
+        <c:axId val="354175024"/>
+        <c:axId val="354176200"/>
+        <c:axId val="356196416"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="100259904"/>
+        <c:axId val="354175024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3747,7 +3719,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100260688"/>
+        <c:crossAx val="354176200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3755,7 +3727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100260688"/>
+        <c:axId val="354176200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -3859,12 +3831,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100259904"/>
+        <c:crossAx val="354175024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="282369208"/>
+        <c:axId val="356196416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3958,7 +3930,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100260688"/>
+        <c:crossAx val="354176200"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -4813,11 +4785,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100256376"/>
-        <c:axId val="100257552"/>
+        <c:axId val="354173456"/>
+        <c:axId val="354173848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100256376"/>
+        <c:axId val="354173456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4923,7 +4895,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100257552"/>
+        <c:crossAx val="354173848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4931,7 +4903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100257552"/>
+        <c:axId val="354173848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.48000000000000004"/>
@@ -5047,7 +5019,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100256376"/>
+        <c:crossAx val="354173456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7609,7 +7581,7 @@
   <dimension ref="A1:AP66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7646,7 +7618,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>4</v>
@@ -7664,25 +7636,25 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="53">
         <v>0.05</v>
       </c>
-      <c r="B2" s="74">
+      <c r="B2" s="60">
         <v>11</v>
       </c>
-      <c r="C2" s="62">
+      <c r="C2" s="63">
         <v>2</v>
       </c>
-      <c r="D2" s="59">
+      <c r="D2" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E2" s="40">
         <v>0.25</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="63">
         <v>2004</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="70">
         <v>182</v>
       </c>
       <c r="H2" s="23">
@@ -7704,22 +7676,22 @@
         <v>0.21835410708760961</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="4">
         <v>23.662715653896385</v>
       </c>
     </row>
     <row r="3" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="41">
         <v>0.5</v>
       </c>
-      <c r="F3" s="63"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="71"/>
       <c r="H3" s="24">
         <v>0.28210000000000002</v>
       </c>
@@ -7739,22 +7711,22 @@
         <v>0.2186278463793149</v>
       </c>
       <c r="N3" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="4">
         <v>25.430628135515548</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="41">
         <v>0.75</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="24">
         <v>0.25430000000000003</v>
       </c>
@@ -7774,22 +7746,22 @@
         <v>0.21617848532292275</v>
       </c>
       <c r="N4" s="45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O4" s="4">
         <v>28.209198735593169</v>
       </c>
     </row>
     <row r="5" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="42">
         <v>1</v>
       </c>
-      <c r="F5" s="63"/>
-      <c r="G5" s="54"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="28">
         <v>0.2366</v>
       </c>
@@ -7809,89 +7781,89 @@
         <v>0.22244895886172322</v>
       </c>
       <c r="N5" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O5" s="4">
         <v>43.46737251627345</v>
       </c>
     </row>
     <row r="6" spans="1:42" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="59">
+      <c r="A6" s="54"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="56">
         <v>0.05</v>
       </c>
       <c r="E6" s="40">
         <v>0.25</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="54"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="71"/>
       <c r="H6" s="29">
         <v>0.35060000000000002</v>
       </c>
       <c r="N6" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O6" s="4">
         <v>22.757402542791436</v>
       </c>
     </row>
     <row r="7" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="41">
         <v>0.5</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="54"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="71"/>
       <c r="H7" s="26">
         <v>0.25330000000000003</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="4">
         <v>25.307875592278492</v>
       </c>
     </row>
     <row r="8" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="72"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="41">
         <v>0.75</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="54"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="24">
         <v>0.25309999999999999</v>
       </c>
       <c r="N8" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O8" s="4">
         <v>25.328987171553045</v>
       </c>
     </row>
     <row r="9" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="64"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="42">
         <v>1</v>
       </c>
-      <c r="F9" s="63"/>
-      <c r="G9" s="54"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="71"/>
       <c r="H9" s="27">
         <v>0.2276</v>
       </c>
       <c r="N9" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O9" s="4">
         <v>35.05863153697296</v>
@@ -7994,17 +7966,17 @@
       </c>
     </row>
     <row r="10" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="60">
+      <c r="A10" s="54"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="59">
         <v>0.1</v>
       </c>
       <c r="E10" s="40">
         <v>0.25</v>
       </c>
-      <c r="F10" s="63"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="29">
         <v>0.22239999999999999</v>
       </c>
@@ -8014,15 +7986,15 @@
       </c>
     </row>
     <row r="11" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="41">
         <v>0.5</v>
       </c>
-      <c r="F11" s="63"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="24">
         <v>0.2162</v>
       </c>
@@ -8032,15 +8004,15 @@
       </c>
     </row>
     <row r="12" spans="1:42" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="41">
         <v>0.75</v>
       </c>
-      <c r="F12" s="63"/>
-      <c r="G12" s="54"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="71"/>
       <c r="H12" s="24">
         <v>0.21859999999999999</v>
       </c>
@@ -8051,15 +8023,15 @@
       </c>
     </row>
     <row r="13" spans="1:42" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="42">
         <v>1</v>
       </c>
-      <c r="F13" s="63"/>
-      <c r="G13" s="54"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="71"/>
       <c r="H13" s="30">
         <v>0.21840000000000001</v>
       </c>
@@ -8081,19 +8053,19 @@
       </c>
     </row>
     <row r="14" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="62">
+      <c r="A14" s="54"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="63">
         <v>5</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E14" s="40">
         <v>0.25</v>
       </c>
-      <c r="F14" s="63"/>
-      <c r="G14" s="54"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="71"/>
       <c r="H14" s="23">
         <v>0.44650000000000001</v>
       </c>
@@ -8118,15 +8090,15 @@
       </c>
     </row>
     <row r="15" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="41">
         <v>0.5</v>
       </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="54"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="71"/>
       <c r="H15" s="24">
         <v>0.27279999999999999</v>
       </c>
@@ -8151,15 +8123,15 @@
       </c>
     </row>
     <row r="16" spans="1:42" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="72"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="41">
         <v>0.75</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="54"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="24">
         <v>0.27</v>
       </c>
@@ -8184,15 +8156,15 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="72"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="42">
         <v>1</v>
       </c>
-      <c r="F17" s="63"/>
-      <c r="G17" s="54"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="27">
         <v>0.23519999999999999</v>
       </c>
@@ -8217,17 +8189,17 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="72"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="59">
+      <c r="A18" s="54"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="56">
         <v>0.05</v>
       </c>
       <c r="E18" s="40">
         <v>0.25</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="54"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="29">
         <v>0.36070000000000002</v>
       </c>
@@ -8237,20 +8209,20 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="72"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="41">
         <v>0.5</v>
       </c>
-      <c r="F19" s="63"/>
-      <c r="G19" s="54"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="71"/>
       <c r="H19" s="24">
         <v>0.24490000000000001</v>
       </c>
       <c r="L19" s="45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N19"/>
       <c r="O19" s="4">
@@ -8258,20 +8230,20 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="41">
         <v>0.75</v>
       </c>
-      <c r="F20" s="63"/>
-      <c r="G20" s="54"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="24">
         <v>0.23669999999999999</v>
       </c>
       <c r="L20" s="45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N20"/>
       <c r="O20" s="4">
@@ -8279,20 +8251,20 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
       <c r="E21" s="42">
         <v>1</v>
       </c>
-      <c r="F21" s="63"/>
-      <c r="G21" s="54"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="71"/>
       <c r="H21" s="27">
         <v>0.25540000000000002</v>
       </c>
       <c r="L21" s="45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N21"/>
       <c r="O21" s="4">
@@ -8300,22 +8272,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="3.5">
-      <c r="A22" s="72"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="60">
+      <c r="A22" s="54"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="59">
         <v>0.1</v>
       </c>
       <c r="E22" s="40">
         <v>0.25</v>
       </c>
-      <c r="F22" s="63"/>
-      <c r="G22" s="54"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="71"/>
       <c r="H22" s="29">
         <v>0.22839999999999999</v>
       </c>
       <c r="L22" s="44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N22"/>
       <c r="O22" s="4">
@@ -8323,15 +8295,15 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="41">
         <v>0.5</v>
       </c>
-      <c r="F23" s="63"/>
-      <c r="G23" s="54"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="71"/>
       <c r="H23" s="24">
         <v>0.2223</v>
       </c>
@@ -8341,15 +8313,15 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="41">
         <v>0.75</v>
       </c>
-      <c r="F24" s="63"/>
-      <c r="G24" s="54"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="71"/>
       <c r="H24" s="24">
         <v>0.2382</v>
       </c>
@@ -8362,15 +8334,15 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="72"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="42">
         <v>1</v>
       </c>
-      <c r="F25" s="64"/>
-      <c r="G25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="28">
         <v>0.21360000000000001</v>
       </c>
@@ -8383,23 +8355,23 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="72"/>
-      <c r="B26" s="77">
+      <c r="A26" s="54"/>
+      <c r="B26" s="64">
         <v>12</v>
       </c>
-      <c r="C26" s="62">
+      <c r="C26" s="63">
         <v>2</v>
       </c>
-      <c r="D26" s="59">
+      <c r="D26" s="56">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E26" s="68">
+      <c r="E26" s="79">
         <v>0.5</v>
       </c>
-      <c r="F26" s="62">
+      <c r="F26" s="63">
         <v>3002</v>
       </c>
-      <c r="G26" s="53">
+      <c r="G26" s="70">
         <v>250</v>
       </c>
       <c r="H26" s="35">
@@ -8415,13 +8387,13 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="54"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="71"/>
       <c r="H27" s="36">
         <f t="shared" si="0"/>
         <v>0.27767733150117957</v>
@@ -8435,13 +8407,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="72"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="55"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="72"/>
       <c r="H28" s="37">
         <f t="shared" si="0"/>
         <v>0.27747258302453448</v>
@@ -8452,17 +8424,17 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="80">
+      <c r="A29" s="54"/>
+      <c r="B29" s="67">
         <v>24</v>
       </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="66">
+      <c r="C29" s="57"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="78">
         <v>3002</v>
       </c>
-      <c r="G29" s="56">
+      <c r="G29" s="73">
         <v>125</v>
       </c>
       <c r="H29" s="29">
@@ -8475,13 +8447,13 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="72"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="54"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="71"/>
       <c r="H30" s="24">
         <f t="shared" si="0"/>
         <v>0.27066461952200482</v>
@@ -8492,13 +8464,13 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="55"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="72"/>
       <c r="H31" s="27">
         <f t="shared" si="0"/>
         <v>0.27348055020385287</v>
@@ -8509,17 +8481,17 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="72"/>
-      <c r="B32" s="80">
+      <c r="A32" s="54"/>
+      <c r="B32" s="67">
         <v>36</v>
       </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="66">
+      <c r="C32" s="57"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="78">
         <v>3026</v>
       </c>
-      <c r="G32" s="56">
+      <c r="G32" s="73">
         <v>84</v>
       </c>
       <c r="H32" s="26">
@@ -8532,13 +8504,13 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="72"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="54"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="71"/>
       <c r="H33" s="24">
         <f t="shared" si="0"/>
         <v>0.27125796408372016</v>
@@ -8549,13 +8521,13 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="73"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="57"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="74"/>
       <c r="H34" s="25">
         <f t="shared" si="0"/>
         <v>0.27194846949300938</v>
@@ -8567,62 +8539,62 @@
     <row r="35" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">
@@ -8630,36 +8602,46 @@
     </row>
     <row r="61" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M61" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M62" s="45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M63" s="45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="13:14" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M64" s="45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="13:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M65" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="13:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="M66" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="G2:G25"/>
+    <mergeCell ref="D26:D34"/>
+    <mergeCell ref="F2:F25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="E26:E34"/>
     <mergeCell ref="A2:A34"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D9"/>
@@ -8674,16 +8656,6 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C26:C34"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="G2:G25"/>
-    <mergeCell ref="D26:D34"/>
-    <mergeCell ref="F2:F25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="E26:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>